<commit_message>
Added More Like This recommendations feature
</commit_message>
<xml_diff>
--- a/flask_api/feature_vec.xlsx
+++ b/flask_api/feature_vec.xlsx
@@ -16,973 +16,973 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="323">
   <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>collard</t>
+  </si>
+  <si>
+    <t>semolina</t>
+  </si>
+  <si>
+    <t>celery</t>
+  </si>
+  <si>
+    <t>chinese yam</t>
+  </si>
+  <si>
+    <t>ranch</t>
+  </si>
+  <si>
+    <t>turkey</t>
+  </si>
+  <si>
+    <t>almond</t>
+  </si>
+  <si>
+    <t>broth</t>
+  </si>
+  <si>
+    <t>norus</t>
+  </si>
+  <si>
+    <t>cabage</t>
+  </si>
+  <si>
+    <t>tempura</t>
+  </si>
+  <si>
+    <t>mayonnaise</t>
+  </si>
+  <si>
     <t>cabbage</t>
   </si>
   <si>
+    <t>yeast</t>
+  </si>
+  <si>
+    <t>snow pea</t>
+  </si>
+  <si>
+    <t>crown daisy</t>
+  </si>
+  <si>
+    <t>crust</t>
+  </si>
+  <si>
+    <t>dinner</t>
+  </si>
+  <si>
+    <t>coloring</t>
+  </si>
+  <si>
+    <t>syrup</t>
+  </si>
+  <si>
+    <t>vegetable</t>
+  </si>
+  <si>
+    <t>alfalfa sprout</t>
+  </si>
+  <si>
+    <t>whipping</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>scallion</t>
+  </si>
+  <si>
+    <t>vanilla</t>
+  </si>
+  <si>
+    <t>pot</t>
+  </si>
+  <si>
+    <t>aonori</t>
+  </si>
+  <si>
+    <t>szechuan</t>
+  </si>
+  <si>
+    <t>spice</t>
+  </si>
+  <si>
+    <t>bean</t>
+  </si>
+  <si>
+    <t>kombu</t>
+  </si>
+  <si>
+    <t>pork</t>
+  </si>
+  <si>
+    <t>garam masala</t>
+  </si>
+  <si>
+    <t>watercre</t>
+  </si>
+  <si>
+    <t>seaweed</t>
+  </si>
+  <si>
+    <t>caramel</t>
+  </si>
+  <si>
+    <t>ice</t>
+  </si>
+  <si>
+    <t>saffron</t>
+  </si>
+  <si>
+    <t>caper</t>
+  </si>
+  <si>
+    <t>saffron thread</t>
+  </si>
+  <si>
+    <t>avocado</t>
+  </si>
+  <si>
+    <t>worcestershire</t>
+  </si>
+  <si>
+    <t>roti</t>
+  </si>
+  <si>
+    <t>cilantro</t>
+  </si>
+  <si>
+    <t>quinoa</t>
+  </si>
+  <si>
+    <t>dulce leche</t>
+  </si>
+  <si>
+    <t>mirin</t>
+  </si>
+  <si>
+    <t>gravy</t>
+  </si>
+  <si>
+    <t>bay</t>
+  </si>
+  <si>
+    <t>spinach</t>
+  </si>
+  <si>
+    <t>tapioca starch</t>
+  </si>
+  <si>
+    <t>oxtail</t>
+  </si>
+  <si>
+    <t>salmon</t>
+  </si>
+  <si>
+    <t>shiso</t>
+  </si>
+  <si>
+    <t>baguette</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>chicken</t>
+  </si>
+  <si>
+    <t>bbq starter</t>
+  </si>
+  <si>
+    <t>carrot</t>
+  </si>
+  <si>
+    <t>dashi</t>
+  </si>
+  <si>
+    <t>shrimp</t>
+  </si>
+  <si>
+    <t>peanut</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>nectar</t>
+  </si>
+  <si>
+    <t>half</t>
+  </si>
+  <si>
+    <t>vinegar</t>
+  </si>
+  <si>
+    <t>chickpea</t>
+  </si>
+  <si>
+    <t>gin</t>
+  </si>
+  <si>
+    <t>hash brown</t>
+  </si>
+  <si>
+    <t>bamboo skewer</t>
+  </si>
+  <si>
+    <t>zucchini</t>
+  </si>
+  <si>
+    <t>hojiso</t>
+  </si>
+  <si>
+    <t>cardamom</t>
+  </si>
+  <si>
+    <t>asparagu</t>
+  </si>
+  <si>
+    <t>prawn</t>
+  </si>
+  <si>
+    <t>sprinkle</t>
+  </si>
+  <si>
+    <t>kelp</t>
+  </si>
+  <si>
+    <t>currant</t>
+  </si>
+  <si>
+    <t>chile</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>gochujang</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>raisin</t>
+  </si>
+  <si>
+    <t>paneer</t>
+  </si>
+  <si>
+    <t>cod</t>
+  </si>
+  <si>
+    <t>pretzel</t>
+  </si>
+  <si>
+    <t>pastum</t>
+  </si>
+  <si>
+    <t>cocoa</t>
+  </si>
+  <si>
+    <t>chipotle</t>
+  </si>
+  <si>
+    <t>paprika</t>
+  </si>
+  <si>
+    <t>lager beer</t>
+  </si>
+  <si>
+    <t>citru</t>
+  </si>
+  <si>
+    <t>fenugreek</t>
+  </si>
+  <si>
+    <t>star anise</t>
+  </si>
+  <si>
+    <t>mascarpone</t>
+  </si>
+  <si>
+    <t>hoisin</t>
+  </si>
+  <si>
+    <t>espresso</t>
+  </si>
+  <si>
+    <t>siracha</t>
+  </si>
+  <si>
+    <t>shallot</t>
+  </si>
+  <si>
+    <t>pecan</t>
+  </si>
+  <si>
+    <t>pepper</t>
+  </si>
+  <si>
+    <t>cookie</t>
+  </si>
+  <si>
+    <t>lukewarm</t>
+  </si>
+  <si>
+    <t>rosemary</t>
+  </si>
+  <si>
+    <t>mace blade</t>
+  </si>
+  <si>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
+    <t>bell pepper</t>
+  </si>
+  <si>
+    <t>piping bags star nozzle</t>
+  </si>
+  <si>
+    <t>coconut</t>
+  </si>
+  <si>
+    <t>ghee</t>
+  </si>
+  <si>
+    <t>pizza dough</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>duck</t>
+  </si>
+  <si>
+    <t>chily</t>
+  </si>
+  <si>
+    <t>side dishes</t>
+  </si>
+  <si>
+    <t>brussels sprout</t>
+  </si>
+  <si>
+    <t>noodle</t>
+  </si>
+  <si>
+    <t>sesame</t>
+  </si>
+  <si>
+    <t>pea</t>
+  </si>
+  <si>
+    <t>tobiko</t>
+  </si>
+  <si>
+    <t>octopu</t>
+  </si>
+  <si>
+    <t>marshmallow</t>
+  </si>
+  <si>
+    <t>perilla</t>
+  </si>
+  <si>
+    <t>gochugaru</t>
+  </si>
+  <si>
+    <t>pistachio</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>boule</t>
+  </si>
+  <si>
+    <t>cucumber</t>
+  </si>
+  <si>
+    <t>ketchup</t>
+  </si>
+  <si>
+    <t>waffle</t>
+  </si>
+  <si>
+    <t>maruchan raman</t>
+  </si>
+  <si>
+    <t>ya mama cajun</t>
+  </si>
+  <si>
+    <t>jalapeno</t>
+  </si>
+  <si>
+    <t>cayenne</t>
+  </si>
+  <si>
+    <t>safron thread</t>
+  </si>
+  <si>
+    <t>equipment</t>
+  </si>
+  <si>
+    <t>bok choy</t>
+  </si>
+  <si>
+    <t>kashmiri</t>
+  </si>
+  <si>
+    <t>kale</t>
+  </si>
+  <si>
+    <t>sausage</t>
+  </si>
+  <si>
+    <t>beetroot</t>
+  </si>
+  <si>
+    <t>tamarind</t>
+  </si>
+  <si>
+    <t>radish</t>
+  </si>
+  <si>
+    <t>wok</t>
+  </si>
+  <si>
+    <t>duck breast</t>
+  </si>
+  <si>
+    <t>goda masala</t>
+  </si>
+  <si>
+    <t>chili</t>
+  </si>
+  <si>
+    <t>sandwich cookies</t>
+  </si>
+  <si>
+    <t>cracker</t>
+  </si>
+  <si>
+    <t>martini glass</t>
+  </si>
+  <si>
+    <t>anchovy</t>
+  </si>
+  <si>
+    <t>baking soda</t>
+  </si>
+  <si>
+    <t>coriander</t>
+  </si>
+  <si>
+    <t>calamari body</t>
+  </si>
+  <si>
+    <t>sambal</t>
+  </si>
+  <si>
+    <t>curry</t>
+  </si>
+  <si>
+    <t>straw</t>
+  </si>
+  <si>
+    <t>bamboo shoot</t>
+  </si>
+  <si>
+    <t>bread</t>
+  </si>
+  <si>
+    <t>aril</t>
+  </si>
+  <si>
+    <t>tonkatsu</t>
+  </si>
+  <si>
+    <t>spaghetti</t>
+  </si>
+  <si>
+    <t>pearl</t>
+  </si>
+  <si>
+    <t>wok spatula</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>wine</t>
+  </si>
+  <si>
+    <t>nutmeg</t>
+  </si>
+  <si>
+    <t>ikura</t>
+  </si>
+  <si>
+    <t>jalapeño</t>
+  </si>
+  <si>
+    <t>daikon</t>
+  </si>
+  <si>
+    <t>sawtooth herb</t>
+  </si>
+  <si>
+    <t>bun</t>
+  </si>
+  <si>
+    <t>pad</t>
+  </si>
+  <si>
+    <t>asian pear</t>
+  </si>
+  <si>
+    <t>chaat masala</t>
+  </si>
+  <si>
+    <t>soy</t>
+  </si>
+  <si>
+    <t>urad</t>
+  </si>
+  <si>
+    <t>puri masala</t>
+  </si>
+  <si>
+    <t>pudding mold</t>
+  </si>
+  <si>
+    <t>doubanjiang</t>
+  </si>
+  <si>
+    <t>skewer</t>
+  </si>
+  <si>
+    <t>bicarbonate soda</t>
+  </si>
+  <si>
+    <t>liqueur</t>
+  </si>
+  <si>
+    <t>dumpling wrapper</t>
+  </si>
+  <si>
+    <t>chive</t>
+  </si>
+  <si>
+    <t>pastry</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>asadetida</t>
+  </si>
+  <si>
+    <t>wasabi</t>
+  </si>
+  <si>
+    <t>thyme</t>
+  </si>
+  <si>
+    <t>oregano</t>
+  </si>
+  <si>
+    <t>bacon</t>
+  </si>
+  <si>
+    <t>mango</t>
+  </si>
+  <si>
+    <t>garnish</t>
+  </si>
+  <si>
+    <t>tea</t>
+  </si>
+  <si>
+    <t>char siu</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>lettuce</t>
+  </si>
+  <si>
+    <t>tonic</t>
+  </si>
+  <si>
+    <t>tamarus</t>
+  </si>
+  <si>
+    <t>kumquat</t>
+  </si>
+  <si>
+    <t>miso</t>
+  </si>
+  <si>
+    <t>pine nut</t>
+  </si>
+  <si>
+    <t>cashew</t>
+  </si>
+  <si>
+    <t>pumpkin</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>masala</t>
+  </si>
+  <si>
+    <t>matcha</t>
+  </si>
+  <si>
+    <t>okra</t>
+  </si>
+  <si>
+    <t>takoyaki turner</t>
+  </si>
+  <si>
+    <t>sourdough baguette</t>
+  </si>
+  <si>
+    <t>clove</t>
+  </si>
+  <si>
+    <t>tartar</t>
+  </si>
+  <si>
+    <t>garlic</t>
+  </si>
+  <si>
+    <t>sage</t>
+  </si>
+  <si>
+    <t>cognac</t>
+  </si>
+  <si>
+    <t>clam</t>
+  </si>
+  <si>
+    <t>takoyaki plate</t>
+  </si>
+  <si>
+    <t>beef</t>
+  </si>
+  <si>
+    <t>flmy</t>
+  </si>
+  <si>
+    <t>cinnamon</t>
+  </si>
+  <si>
+    <t>pâté</t>
+  </si>
+  <si>
+    <t>berry</t>
+  </si>
+  <si>
+    <t>jeera</t>
+  </si>
+  <si>
+    <t>galangal</t>
+  </si>
+  <si>
+    <t>tuna</t>
+  </si>
+  <si>
+    <t>guacamole</t>
+  </si>
+  <si>
+    <t>prosciutto</t>
+  </si>
+  <si>
+    <t>cilantro stem</t>
+  </si>
+  <si>
+    <t>broccoli</t>
+  </si>
+  <si>
+    <t>marinara</t>
+  </si>
+  <si>
+    <t>mackerel</t>
+  </si>
+  <si>
+    <t>winter citru</t>
+  </si>
+  <si>
+    <t>oyster</t>
+  </si>
+  <si>
+    <t>korma</t>
+  </si>
+  <si>
+    <t>crab</t>
+  </si>
+  <si>
+    <t>asafoetida</t>
+  </si>
+  <si>
+    <t>bamboo shoot strip</t>
+  </si>
+  <si>
+    <t>taro</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>crescent dinner</t>
+  </si>
+  <si>
+    <t>sunflower</t>
+  </si>
+  <si>
     <t>allspice</t>
   </si>
   <si>
-    <t>mirin</t>
+    <t>quality sichuan</t>
+  </si>
+  <si>
+    <t>gelatin</t>
+  </si>
+  <si>
+    <t>anise</t>
+  </si>
+  <si>
+    <t>tomato</t>
+  </si>
+  <si>
+    <t>chilli</t>
+  </si>
+  <si>
+    <t>nori furikake</t>
+  </si>
+  <si>
+    <t>smoke</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>chana dal</t>
+  </si>
+  <si>
+    <t>sushigrade sea urchin</t>
+  </si>
+  <si>
+    <t>tofu</t>
+  </si>
+  <si>
+    <t>turmeric</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>baking</t>
+  </si>
+  <si>
+    <t>spice grinder</t>
+  </si>
+  <si>
+    <t>oat</t>
+  </si>
+  <si>
+    <t>parsley</t>
+  </si>
+  <si>
+    <t>sudachi</t>
+  </si>
+  <si>
+    <t>edamame</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>dumplings broth</t>
+  </si>
+  <si>
+    <t>butter</t>
+  </si>
+  <si>
+    <t>mini pretzel</t>
+  </si>
+  <si>
+    <t>fennel</t>
+  </si>
+  <si>
+    <t>candy</t>
+  </si>
+  <si>
+    <t>biscuit</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>wonton wrapper</t>
+  </si>
+  <si>
+    <t>kimchi</t>
+  </si>
+  <si>
+    <t>french</t>
+  </si>
+  <si>
+    <t>mustard</t>
+  </si>
+  <si>
+    <t>bisto</t>
+  </si>
+  <si>
+    <t>roe</t>
+  </si>
+  <si>
+    <t>wrapper</t>
+  </si>
+  <si>
+    <t>honey</t>
+  </si>
+  <si>
+    <t>chocolate</t>
+  </si>
+  <si>
+    <t>mushroom</t>
+  </si>
+  <si>
+    <t>alfredo</t>
+  </si>
+  <si>
+    <t>sichuan</t>
+  </si>
+  <si>
+    <t>flour</t>
+  </si>
+  <si>
+    <t>cauliflower</t>
+  </si>
+  <si>
+    <t>grapefruit</t>
+  </si>
+  <si>
+    <t>kiwi</t>
+  </si>
+  <si>
+    <t>tortilla</t>
+  </si>
+  <si>
+    <t>wooden chopstick</t>
+  </si>
+  <si>
+    <t>yogurt</t>
   </si>
   <si>
     <t>nori</t>
   </si>
   <si>
-    <t>sudachi</t>
-  </si>
-  <si>
-    <t>sesame</t>
-  </si>
-  <si>
-    <t>whipping</t>
-  </si>
-  <si>
-    <t>cocoa</t>
+    <t>salsa</t>
+  </si>
+  <si>
+    <t>katsuobushi</t>
+  </si>
+  <si>
+    <t>rib</t>
+  </si>
+  <si>
+    <t>duck carcas</t>
+  </si>
+  <si>
+    <t>tandoori side dish</t>
+  </si>
+  <si>
+    <t>paratha</t>
+  </si>
+  <si>
+    <t>cumin</t>
+  </si>
+  <si>
+    <t>sugar</t>
+  </si>
+  <si>
+    <t>bonito dashi</t>
   </si>
   <si>
     <t>arugula</t>
   </si>
   <si>
-    <t>half</t>
-  </si>
-  <si>
-    <t>puri masala</t>
-  </si>
-  <si>
-    <t>duck</t>
+    <t>spaghettus</t>
+  </si>
+  <si>
+    <t>mint</t>
+  </si>
+  <si>
+    <t>muffin tin</t>
+  </si>
+  <si>
+    <t>garlic naan</t>
+  </si>
+  <si>
+    <t>takoyaki</t>
+  </si>
+  <si>
+    <t>elaichi</t>
+  </si>
+  <si>
+    <t>tangerine</t>
+  </si>
+  <si>
+    <t>ginger</t>
+  </si>
+  <si>
+    <t>squash</t>
+  </si>
+  <si>
+    <t>iron skillet</t>
+  </si>
+  <si>
+    <t>franks</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>ham</t>
+  </si>
+  <si>
+    <t>fusilli</t>
+  </si>
+  <si>
+    <t>basil</t>
+  </si>
+  <si>
+    <t>matzo</t>
+  </si>
+  <si>
+    <t>dill</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>halibut</t>
   </si>
   <si>
     <t>fudge</t>
-  </si>
-  <si>
-    <t>bay</t>
-  </si>
-  <si>
-    <t>dog</t>
-  </si>
-  <si>
-    <t>quinoa</t>
-  </si>
-  <si>
-    <t>lukewarm</t>
-  </si>
-  <si>
-    <t>french</t>
-  </si>
-  <si>
-    <t>vinegar</t>
-  </si>
-  <si>
-    <t>oxtail</t>
-  </si>
-  <si>
-    <t>bread</t>
-  </si>
-  <si>
-    <t>shrimp</t>
-  </si>
-  <si>
-    <t>butter</t>
-  </si>
-  <si>
-    <t>beer</t>
-  </si>
-  <si>
-    <t>sambal</t>
-  </si>
-  <si>
-    <t>yogurt</t>
-  </si>
-  <si>
-    <t>cookie</t>
-  </si>
-  <si>
-    <t>syrup</t>
-  </si>
-  <si>
-    <t>garam masala</t>
-  </si>
-  <si>
-    <t>roe</t>
-  </si>
-  <si>
-    <t>kimchi</t>
-  </si>
-  <si>
-    <t>sushigrade sea urchin</t>
-  </si>
-  <si>
-    <t>tea</t>
-  </si>
-  <si>
-    <t>asparagu</t>
-  </si>
-  <si>
-    <t>masala</t>
-  </si>
-  <si>
-    <t>cauliflower</t>
-  </si>
-  <si>
-    <t>halibut</t>
-  </si>
-  <si>
-    <t>roti</t>
-  </si>
-  <si>
-    <t>oregano</t>
-  </si>
-  <si>
-    <t>avocado</t>
-  </si>
-  <si>
-    <t>kale</t>
-  </si>
-  <si>
-    <t>celery</t>
-  </si>
-  <si>
-    <t>dashi</t>
-  </si>
-  <si>
-    <t>tapioca starch</t>
-  </si>
-  <si>
-    <t>marinara</t>
-  </si>
-  <si>
-    <t>spaghetti</t>
-  </si>
-  <si>
-    <t>guacamole</t>
-  </si>
-  <si>
-    <t>ice</t>
-  </si>
-  <si>
-    <t>sprinkle</t>
-  </si>
-  <si>
-    <t>sugar</t>
-  </si>
-  <si>
-    <t>pearl</t>
-  </si>
-  <si>
-    <t>chili</t>
-  </si>
-  <si>
-    <t>salmon</t>
-  </si>
-  <si>
-    <t>tobiko</t>
-  </si>
-  <si>
-    <t>cashew</t>
-  </si>
-  <si>
-    <t>muffin tin</t>
-  </si>
-  <si>
-    <t>sunflower</t>
-  </si>
-  <si>
-    <t>bamboo skewer</t>
-  </si>
-  <si>
-    <t>garnish</t>
-  </si>
-  <si>
-    <t>rosemary</t>
-  </si>
-  <si>
-    <t>apple</t>
-  </si>
-  <si>
-    <t>espresso</t>
-  </si>
-  <si>
-    <t>takoyaki plate</t>
-  </si>
-  <si>
-    <t>broth</t>
-  </si>
-  <si>
-    <t>coconut</t>
-  </si>
-  <si>
-    <t>salt</t>
-  </si>
-  <si>
-    <t>kelp</t>
-  </si>
-  <si>
-    <t>norus</t>
-  </si>
-  <si>
-    <t>lime</t>
-  </si>
-  <si>
-    <t>alfredo</t>
-  </si>
-  <si>
-    <t>chinese yam</t>
-  </si>
-  <si>
-    <t>dinner</t>
-  </si>
-  <si>
-    <t>fusilli</t>
-  </si>
-  <si>
-    <t>jeera</t>
-  </si>
-  <si>
-    <t>cilantro</t>
-  </si>
-  <si>
-    <t>ya mama cajun</t>
-  </si>
-  <si>
-    <t>chocolate</t>
-  </si>
-  <si>
-    <t>okra</t>
-  </si>
-  <si>
-    <t>waffle</t>
-  </si>
-  <si>
-    <t>salsa</t>
-  </si>
-  <si>
-    <t>biscuit</t>
-  </si>
-  <si>
-    <t>lemon</t>
-  </si>
-  <si>
-    <t>bird</t>
-  </si>
-  <si>
-    <t>cilantro stem</t>
-  </si>
-  <si>
-    <t>mace blade</t>
-  </si>
-  <si>
-    <t>kiwi</t>
-  </si>
-  <si>
-    <t>almond</t>
-  </si>
-  <si>
-    <t>pizza dough</t>
-  </si>
-  <si>
-    <t>katsuobushi</t>
-  </si>
-  <si>
-    <t>star</t>
-  </si>
-  <si>
-    <t>asian pear</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>mascarpone</t>
-  </si>
-  <si>
-    <t>martini glass</t>
-  </si>
-  <si>
-    <t>tamarind</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-  <si>
-    <t>korma</t>
-  </si>
-  <si>
-    <t>star anise</t>
-  </si>
-  <si>
-    <t>paneer</t>
-  </si>
-  <si>
-    <t>shallot</t>
-  </si>
-  <si>
-    <t>chive</t>
-  </si>
-  <si>
-    <t>spice</t>
-  </si>
-  <si>
-    <t>snow pea</t>
-  </si>
-  <si>
-    <t>bok choy</t>
-  </si>
-  <si>
-    <t>cracker</t>
-  </si>
-  <si>
-    <t>aonori</t>
-  </si>
-  <si>
-    <t>asadetida</t>
-  </si>
-  <si>
-    <t>clove</t>
-  </si>
-  <si>
-    <t>fennel</t>
-  </si>
-  <si>
-    <t>gin</t>
-  </si>
-  <si>
-    <t>spice grinder</t>
-  </si>
-  <si>
-    <t>pad</t>
-  </si>
-  <si>
-    <t>bamboo shoot strip</t>
-  </si>
-  <si>
-    <t>mustard</t>
-  </si>
-  <si>
-    <t>cod</t>
-  </si>
-  <si>
-    <t>takoyaki turner</t>
-  </si>
-  <si>
-    <t>crown daisy</t>
-  </si>
-  <si>
-    <t>skewer</t>
-  </si>
-  <si>
-    <t>sandwich cookies</t>
-  </si>
-  <si>
-    <t>mackerel</t>
-  </si>
-  <si>
-    <t>nori furikake</t>
-  </si>
-  <si>
-    <t>lager beer</t>
-  </si>
-  <si>
-    <t>piping bags star nozzle</t>
-  </si>
-  <si>
-    <t>tandoori side dish</t>
-  </si>
-  <si>
-    <t>turmeric</t>
-  </si>
-  <si>
-    <t>dumplings broth</t>
-  </si>
-  <si>
-    <t>corn</t>
-  </si>
-  <si>
-    <t>kashmiri</t>
-  </si>
-  <si>
-    <t>bbq starter</t>
-  </si>
-  <si>
-    <t>pastry</t>
-  </si>
-  <si>
-    <t>chickpea</t>
-  </si>
-  <si>
-    <t>bonito dashi</t>
-  </si>
-  <si>
-    <t>gochugaru</t>
-  </si>
-  <si>
-    <t>bisto</t>
-  </si>
-  <si>
-    <t>matzo</t>
-  </si>
-  <si>
-    <t>prawn</t>
-  </si>
-  <si>
-    <t>aril</t>
-  </si>
-  <si>
-    <t>vanilla</t>
-  </si>
-  <si>
-    <t>tonic</t>
-  </si>
-  <si>
-    <t>caramel</t>
-  </si>
-  <si>
-    <t>beetroot</t>
-  </si>
-  <si>
-    <t>collard</t>
-  </si>
-  <si>
-    <t>paratha</t>
-  </si>
-  <si>
-    <t>chicken</t>
-  </si>
-  <si>
-    <t>matcha</t>
-  </si>
-  <si>
-    <t>cake</t>
-  </si>
-  <si>
-    <t>scallion</t>
-  </si>
-  <si>
-    <t>asafoetida</t>
-  </si>
-  <si>
-    <t>wok</t>
-  </si>
-  <si>
-    <t>char siu</t>
-  </si>
-  <si>
-    <t>turkey</t>
-  </si>
-  <si>
-    <t>curry</t>
-  </si>
-  <si>
-    <t>chipotle</t>
-  </si>
-  <si>
-    <t>doubanjiang</t>
-  </si>
-  <si>
-    <t>peanut</t>
-  </si>
-  <si>
-    <t>mayonnaise</t>
-  </si>
-  <si>
-    <t>mango</t>
-  </si>
-  <si>
-    <t>kombu</t>
-  </si>
-  <si>
-    <t>bicarbonate soda</t>
-  </si>
-  <si>
-    <t>bamboo shoot</t>
-  </si>
-  <si>
-    <t>anchovy</t>
-  </si>
-  <si>
-    <t>chile</t>
-  </si>
-  <si>
-    <t>dulce leche</t>
-  </si>
-  <si>
-    <t>oil</t>
-  </si>
-  <si>
-    <t>liqueur</t>
-  </si>
-  <si>
-    <t>wine</t>
-  </si>
-  <si>
-    <t>garlic naan</t>
-  </si>
-  <si>
-    <t>banana</t>
-  </si>
-  <si>
-    <t>nectar</t>
-  </si>
-  <si>
-    <t>pork</t>
-  </si>
-  <si>
-    <t>alfalfa sprout</t>
-  </si>
-  <si>
-    <t>egg</t>
-  </si>
-  <si>
-    <t>straw</t>
-  </si>
-  <si>
-    <t>franks</t>
-  </si>
-  <si>
-    <t>flour</t>
-  </si>
-  <si>
-    <t>perilla</t>
-  </si>
-  <si>
-    <t>garlic</t>
-  </si>
-  <si>
-    <t>sawtooth herb</t>
-  </si>
-  <si>
-    <t>daikon</t>
-  </si>
-  <si>
-    <t>cucumber</t>
-  </si>
-  <si>
-    <t>duck carcas</t>
-  </si>
-  <si>
-    <t>pretzel</t>
-  </si>
-  <si>
-    <t>szechuan</t>
-  </si>
-  <si>
-    <t>safron thread</t>
-  </si>
-  <si>
-    <t>pistachio</t>
-  </si>
-  <si>
-    <t>clam</t>
-  </si>
-  <si>
-    <t>elaichi</t>
-  </si>
-  <si>
-    <t>spaghettus</t>
-  </si>
-  <si>
-    <t>baking soda</t>
-  </si>
-  <si>
-    <t>mini pretzel</t>
-  </si>
-  <si>
-    <t>edamame</t>
-  </si>
-  <si>
-    <t>pudding mold</t>
-  </si>
-  <si>
-    <t>maruchan raman</t>
-  </si>
-  <si>
-    <t>crab</t>
-  </si>
-  <si>
-    <t>caper</t>
-  </si>
-  <si>
-    <t>duck breast</t>
-  </si>
-  <si>
-    <t>pumpkin</t>
-  </si>
-  <si>
-    <t>milk</t>
-  </si>
-  <si>
-    <t>cardamom</t>
-  </si>
-  <si>
-    <t>worcestershire</t>
-  </si>
-  <si>
-    <t>chana dal</t>
-  </si>
-  <si>
-    <t>rice</t>
-  </si>
-  <si>
-    <t>anise</t>
-  </si>
-  <si>
-    <t>currant</t>
-  </si>
-  <si>
-    <t>pea</t>
-  </si>
-  <si>
-    <t>ginger</t>
-  </si>
-  <si>
-    <t>pastum</t>
-  </si>
-  <si>
-    <t>ranch</t>
-  </si>
-  <si>
-    <t>goda masala</t>
-  </si>
-  <si>
-    <t>marshmallow</t>
-  </si>
-  <si>
-    <t>spinach</t>
-  </si>
-  <si>
-    <t>raisin</t>
-  </si>
-  <si>
-    <t>pot</t>
-  </si>
-  <si>
-    <t>tamarus</t>
-  </si>
-  <si>
-    <t>saffron</t>
-  </si>
-  <si>
-    <t>gochujang</t>
-  </si>
-  <si>
-    <t>ham</t>
-  </si>
-  <si>
-    <t>hoisin</t>
-  </si>
-  <si>
-    <t>chilli</t>
-  </si>
-  <si>
-    <t>semolina</t>
-  </si>
-  <si>
-    <t>hash brown</t>
-  </si>
-  <si>
-    <t>nutmeg</t>
-  </si>
-  <si>
-    <t>paprika</t>
-  </si>
-  <si>
-    <t>oat</t>
-  </si>
-  <si>
-    <t>cinnamon</t>
-  </si>
-  <si>
-    <t>watercre</t>
-  </si>
-  <si>
-    <t>basil</t>
-  </si>
-  <si>
-    <t>smoke</t>
-  </si>
-  <si>
-    <t>tortilla</t>
-  </si>
-  <si>
-    <t>wrapper</t>
-  </si>
-  <si>
-    <t>onion</t>
-  </si>
-  <si>
-    <t>jalapeno</t>
-  </si>
-  <si>
-    <t>jalapeño</t>
-  </si>
-  <si>
-    <t>galangal</t>
-  </si>
-  <si>
-    <t>tartar</t>
-  </si>
-  <si>
-    <t>mushroom</t>
-  </si>
-  <si>
-    <t>thyme</t>
-  </si>
-  <si>
-    <t>dumpling wrapper</t>
-  </si>
-  <si>
-    <t>flmy</t>
-  </si>
-  <si>
-    <t>wok spatula</t>
-  </si>
-  <si>
-    <t>octopu</t>
-  </si>
-  <si>
-    <t>cayenne</t>
-  </si>
-  <si>
-    <t>tonkatsu</t>
-  </si>
-  <si>
-    <t>iron skillet</t>
-  </si>
-  <si>
-    <t>equipment</t>
-  </si>
-  <si>
-    <t>tangerine</t>
-  </si>
-  <si>
-    <t>urad</t>
-  </si>
-  <si>
-    <t>wooden chopstick</t>
-  </si>
-  <si>
-    <t>baking</t>
-  </si>
-  <si>
-    <t>bacon</t>
-  </si>
-  <si>
-    <t>ghee</t>
-  </si>
-  <si>
-    <t>fenugreek</t>
-  </si>
-  <si>
-    <t>quality sichuan</t>
-  </si>
-  <si>
-    <t>pecan</t>
-  </si>
-  <si>
-    <t>dill</t>
-  </si>
-  <si>
-    <t>bean</t>
-  </si>
-  <si>
-    <t>siracha</t>
-  </si>
-  <si>
-    <t>tempura</t>
-  </si>
-  <si>
-    <t>sichuan</t>
-  </si>
-  <si>
-    <t>brussels sprout</t>
-  </si>
-  <si>
-    <t>cabage</t>
-  </si>
-  <si>
-    <t>winter citru</t>
-  </si>
-  <si>
-    <t>crescent dinner</t>
-  </si>
-  <si>
-    <t>side dishes</t>
-  </si>
-  <si>
-    <t>mint</t>
-  </si>
-  <si>
-    <t>cumin</t>
-  </si>
-  <si>
-    <t>taro</t>
-  </si>
-  <si>
-    <t>pine nut</t>
-  </si>
-  <si>
-    <t>sausage</t>
-  </si>
-  <si>
-    <t>bun</t>
-  </si>
-  <si>
-    <t>seaweed</t>
-  </si>
-  <si>
-    <t>ketchup</t>
-  </si>
-  <si>
-    <t>boule</t>
-  </si>
-  <si>
-    <t>sourdough baguette</t>
-  </si>
-  <si>
-    <t>citru</t>
-  </si>
-  <si>
-    <t>hojiso</t>
-  </si>
-  <si>
-    <t>berry</t>
-  </si>
-  <si>
-    <t>wonton wrapper</t>
-  </si>
-  <si>
-    <t>calamari body</t>
-  </si>
-  <si>
-    <t>gelatin</t>
-  </si>
-  <si>
-    <t>oyster</t>
-  </si>
-  <si>
-    <t>tuna</t>
-  </si>
-  <si>
-    <t>potato</t>
-  </si>
-  <si>
-    <t>beef</t>
-  </si>
-  <si>
-    <t>kumquat</t>
-  </si>
-  <si>
-    <t>miso</t>
-  </si>
-  <si>
-    <t>zucchini</t>
-  </si>
-  <si>
-    <t>lettuce</t>
-  </si>
-  <si>
-    <t>crust</t>
-  </si>
-  <si>
-    <t>honey</t>
-  </si>
-  <si>
-    <t>wasabi</t>
-  </si>
-  <si>
-    <t>broccoli</t>
-  </si>
-  <si>
-    <t>pepper</t>
-  </si>
-  <si>
-    <t>chaat masala</t>
-  </si>
-  <si>
-    <t>saffron thread</t>
-  </si>
-  <si>
-    <t>squash</t>
-  </si>
-  <si>
-    <t>sage</t>
-  </si>
-  <si>
-    <t>yeast</t>
-  </si>
-  <si>
-    <t>rib</t>
-  </si>
-  <si>
-    <t>vegetable</t>
-  </si>
-  <si>
-    <t>pâté</t>
-  </si>
-  <si>
-    <t>gravy</t>
-  </si>
-  <si>
-    <t>takoyaki</t>
-  </si>
-  <si>
-    <t>tomato</t>
-  </si>
-  <si>
-    <t>grapefruit</t>
-  </si>
-  <si>
-    <t>coriander</t>
-  </si>
-  <si>
-    <t>ikura</t>
-  </si>
-  <si>
-    <t>candy</t>
-  </si>
-  <si>
-    <t>cognac</t>
-  </si>
-  <si>
-    <t>tofu</t>
-  </si>
-  <si>
-    <t>coffee</t>
-  </si>
-  <si>
-    <t>baguette</t>
-  </si>
-  <si>
-    <t>bell pepper</t>
-  </si>
-  <si>
-    <t>radish</t>
-  </si>
-  <si>
-    <t>prosciutto</t>
-  </si>
-  <si>
-    <t>shiso</t>
-  </si>
-  <si>
-    <t>coloring</t>
-  </si>
-  <si>
-    <t>parsley</t>
-  </si>
-  <si>
-    <t>noodle</t>
-  </si>
-  <si>
-    <t>carrot</t>
-  </si>
-  <si>
-    <t>soy</t>
-  </si>
-  <si>
-    <t>cheese</t>
-  </si>
-  <si>
-    <t>chily</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1364,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1380,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1396,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1404,7 +1404,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1412,7 +1412,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1420,7 +1420,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1428,7 +1428,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1452,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1460,7 +1460,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1468,7 +1468,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1492,7 +1492,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1500,7 +1500,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1508,7 +1508,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1516,7 +1516,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1524,7 +1524,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1532,7 +1532,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1556,7 +1556,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1564,7 +1564,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1572,7 +1572,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1580,7 +1580,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1588,7 +1588,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1604,7 +1604,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1612,7 +1612,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1620,7 +1620,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1628,7 +1628,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1636,7 +1636,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1644,7 +1644,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1660,7 +1660,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1668,7 +1668,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1684,7 +1684,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1692,7 +1692,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1700,7 +1700,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1708,7 +1708,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1716,7 +1716,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1732,7 +1732,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1740,7 +1740,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1748,7 +1748,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1756,7 +1756,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1764,7 +1764,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1772,7 +1772,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1788,7 +1788,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1796,7 +1796,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1812,7 +1812,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1820,7 +1820,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1828,7 +1828,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1836,7 +1836,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1852,7 +1852,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1860,7 +1860,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1868,7 +1868,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1876,7 +1876,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>137</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1884,7 +1884,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1892,7 +1892,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1900,7 +1900,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1924,7 +1924,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1932,7 +1932,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1948,7 +1948,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1964,7 +1964,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1972,7 +1972,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1996,7 +1996,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2004,7 +2004,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2012,7 +2012,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2052,7 +2052,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2068,7 +2068,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2076,7 +2076,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2084,7 +2084,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2116,7 +2116,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2132,7 +2132,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2140,7 +2140,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2148,7 +2148,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2156,7 +2156,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2164,7 +2164,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2172,7 +2172,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>93</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2180,7 +2180,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2196,7 +2196,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2204,7 +2204,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2212,7 +2212,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>14</v>
+        <v>99</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2220,7 +2220,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2228,7 +2228,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2236,7 +2236,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2244,7 +2244,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2252,7 +2252,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2260,7 +2260,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2268,7 +2268,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2284,7 +2284,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2292,7 +2292,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2308,7 +2308,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2316,7 +2316,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>58</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2324,7 +2324,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2340,7 +2340,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2348,7 +2348,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2356,7 +2356,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2364,7 +2364,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2372,7 +2372,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2380,7 +2380,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>77</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2388,7 +2388,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2396,7 +2396,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2404,7 +2404,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2444,7 +2444,7 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2452,7 +2452,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2468,7 +2468,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2476,7 +2476,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2492,7 +2492,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2500,7 +2500,7 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2508,7 +2508,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2516,7 +2516,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2524,7 +2524,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2548,7 +2548,7 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2556,7 +2556,7 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2564,7 +2564,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2580,7 +2580,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2596,7 +2596,7 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2604,7 +2604,7 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2620,7 +2620,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2636,7 +2636,7 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2644,7 +2644,7 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2660,7 +2660,7 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2676,7 +2676,7 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2692,7 +2692,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2700,7 +2700,7 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2708,7 +2708,7 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2724,7 +2724,7 @@
         <v>171</v>
       </c>
       <c r="B173">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2732,7 +2732,7 @@
         <v>172</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2740,7 +2740,7 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2748,7 +2748,7 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2756,7 +2756,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2764,7 +2764,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>108</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2780,7 +2780,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2788,7 +2788,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2820,7 +2820,7 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2828,7 +2828,7 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2852,7 +2852,7 @@
         <v>187</v>
       </c>
       <c r="B189">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -2860,7 +2860,7 @@
         <v>188</v>
       </c>
       <c r="B190">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -2868,7 +2868,7 @@
         <v>189</v>
       </c>
       <c r="B191">
-        <v>1</v>
+        <v>137</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2884,7 +2884,7 @@
         <v>191</v>
       </c>
       <c r="B193">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -2892,7 +2892,7 @@
         <v>192</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -2900,7 +2900,7 @@
         <v>193</v>
       </c>
       <c r="B195">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2908,7 +2908,7 @@
         <v>194</v>
       </c>
       <c r="B196">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2916,7 +2916,7 @@
         <v>195</v>
       </c>
       <c r="B197">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2924,7 +2924,7 @@
         <v>196</v>
       </c>
       <c r="B198">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2932,7 +2932,7 @@
         <v>197</v>
       </c>
       <c r="B199">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2940,7 +2940,7 @@
         <v>198</v>
       </c>
       <c r="B200">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2948,7 +2948,7 @@
         <v>199</v>
       </c>
       <c r="B201">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2956,7 +2956,7 @@
         <v>200</v>
       </c>
       <c r="B202">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2964,7 +2964,7 @@
         <v>201</v>
       </c>
       <c r="B203">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2972,7 +2972,7 @@
         <v>202</v>
       </c>
       <c r="B204">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2988,7 +2988,7 @@
         <v>204</v>
       </c>
       <c r="B206">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2996,7 +2996,7 @@
         <v>205</v>
       </c>
       <c r="B207">
-        <v>71</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -3004,7 +3004,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -3012,7 +3012,7 @@
         <v>207</v>
       </c>
       <c r="B209">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -3028,7 +3028,7 @@
         <v>209</v>
       </c>
       <c r="B211">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3036,7 +3036,7 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -3060,7 +3060,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -3068,7 +3068,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -3076,7 +3076,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -3084,7 +3084,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>5</v>
+        <v>108</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -3092,7 +3092,7 @@
         <v>217</v>
       </c>
       <c r="B219">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -3100,7 +3100,7 @@
         <v>218</v>
       </c>
       <c r="B220">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -3124,7 +3124,7 @@
         <v>221</v>
       </c>
       <c r="B223">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -3132,7 +3132,7 @@
         <v>222</v>
       </c>
       <c r="B224">
-        <v>14</v>
+        <v>63</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -3140,7 +3140,7 @@
         <v>223</v>
       </c>
       <c r="B225">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -3148,7 +3148,7 @@
         <v>224</v>
       </c>
       <c r="B226">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -3156,7 +3156,7 @@
         <v>225</v>
       </c>
       <c r="B227">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -3164,7 +3164,7 @@
         <v>226</v>
       </c>
       <c r="B228">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -3172,7 +3172,7 @@
         <v>227</v>
       </c>
       <c r="B229">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -3180,7 +3180,7 @@
         <v>228</v>
       </c>
       <c r="B230">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -3196,7 +3196,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -3204,7 +3204,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -3212,7 +3212,7 @@
         <v>232</v>
       </c>
       <c r="B234">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -3220,7 +3220,7 @@
         <v>233</v>
       </c>
       <c r="B235">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -3236,7 +3236,7 @@
         <v>235</v>
       </c>
       <c r="B237">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -3244,7 +3244,7 @@
         <v>236</v>
       </c>
       <c r="B238">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -3260,7 +3260,7 @@
         <v>238</v>
       </c>
       <c r="B240">
-        <v>63</v>
+        <v>2</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -3284,7 +3284,7 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -3292,7 +3292,7 @@
         <v>242</v>
       </c>
       <c r="B244">
-        <v>1</v>
+        <v>120</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -3316,7 +3316,7 @@
         <v>245</v>
       </c>
       <c r="B247">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -3332,7 +3332,7 @@
         <v>247</v>
       </c>
       <c r="B249">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -3340,7 +3340,7 @@
         <v>248</v>
       </c>
       <c r="B250">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -3348,7 +3348,7 @@
         <v>249</v>
       </c>
       <c r="B251">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -3356,7 +3356,7 @@
         <v>250</v>
       </c>
       <c r="B252">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -3364,7 +3364,7 @@
         <v>251</v>
       </c>
       <c r="B253">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -3380,7 +3380,7 @@
         <v>253</v>
       </c>
       <c r="B255">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -3388,7 +3388,7 @@
         <v>254</v>
       </c>
       <c r="B256">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -3396,7 +3396,7 @@
         <v>255</v>
       </c>
       <c r="B257">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -3404,7 +3404,7 @@
         <v>256</v>
       </c>
       <c r="B258">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -3412,7 +3412,7 @@
         <v>257</v>
       </c>
       <c r="B259">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -3420,7 +3420,7 @@
         <v>258</v>
       </c>
       <c r="B260">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -3428,7 +3428,7 @@
         <v>259</v>
       </c>
       <c r="B261">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -3436,7 +3436,7 @@
         <v>260</v>
       </c>
       <c r="B262">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -3452,7 +3452,7 @@
         <v>262</v>
       </c>
       <c r="B264">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -3468,7 +3468,7 @@
         <v>264</v>
       </c>
       <c r="B266">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -3476,7 +3476,7 @@
         <v>265</v>
       </c>
       <c r="B267">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -3492,7 +3492,7 @@
         <v>267</v>
       </c>
       <c r="B269">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -3500,7 +3500,7 @@
         <v>268</v>
       </c>
       <c r="B270">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -3508,7 +3508,7 @@
         <v>269</v>
       </c>
       <c r="B271">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -3516,7 +3516,7 @@
         <v>270</v>
       </c>
       <c r="B272">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -3524,7 +3524,7 @@
         <v>271</v>
       </c>
       <c r="B273">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -3532,7 +3532,7 @@
         <v>272</v>
       </c>
       <c r="B274">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -3540,7 +3540,7 @@
         <v>273</v>
       </c>
       <c r="B275">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -3548,7 +3548,7 @@
         <v>274</v>
       </c>
       <c r="B276">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -3556,7 +3556,7 @@
         <v>275</v>
       </c>
       <c r="B277">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -3564,7 +3564,7 @@
         <v>276</v>
       </c>
       <c r="B278">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -3572,7 +3572,7 @@
         <v>277</v>
       </c>
       <c r="B279">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -3580,7 +3580,7 @@
         <v>278</v>
       </c>
       <c r="B280">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -3588,7 +3588,7 @@
         <v>279</v>
       </c>
       <c r="B281">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -3596,7 +3596,7 @@
         <v>280</v>
       </c>
       <c r="B282">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -3604,7 +3604,7 @@
         <v>281</v>
       </c>
       <c r="B283">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -3612,7 +3612,7 @@
         <v>282</v>
       </c>
       <c r="B284">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -3620,7 +3620,7 @@
         <v>283</v>
       </c>
       <c r="B285">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -3628,7 +3628,7 @@
         <v>284</v>
       </c>
       <c r="B286">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -3636,7 +3636,7 @@
         <v>285</v>
       </c>
       <c r="B287">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -3644,7 +3644,7 @@
         <v>286</v>
       </c>
       <c r="B288">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -3652,7 +3652,7 @@
         <v>287</v>
       </c>
       <c r="B289">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -3668,7 +3668,7 @@
         <v>289</v>
       </c>
       <c r="B291">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -3676,7 +3676,7 @@
         <v>290</v>
       </c>
       <c r="B292">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -3684,7 +3684,7 @@
         <v>291</v>
       </c>
       <c r="B293">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -3692,7 +3692,7 @@
         <v>292</v>
       </c>
       <c r="B294">
-        <v>93</v>
+        <v>4</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -3716,7 +3716,7 @@
         <v>295</v>
       </c>
       <c r="B297">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -3724,7 +3724,7 @@
         <v>296</v>
       </c>
       <c r="B298">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -3732,7 +3732,7 @@
         <v>297</v>
       </c>
       <c r="B299">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -3748,7 +3748,7 @@
         <v>299</v>
       </c>
       <c r="B301">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -3756,7 +3756,7 @@
         <v>300</v>
       </c>
       <c r="B302">
-        <v>1</v>
+        <v>117</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -3780,7 +3780,7 @@
         <v>303</v>
       </c>
       <c r="B305">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -3788,7 +3788,7 @@
         <v>304</v>
       </c>
       <c r="B306">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -3796,7 +3796,7 @@
         <v>305</v>
       </c>
       <c r="B307">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -3828,7 +3828,7 @@
         <v>309</v>
       </c>
       <c r="B311">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -3836,7 +3836,7 @@
         <v>310</v>
       </c>
       <c r="B312">
-        <v>2</v>
+        <v>71</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -3844,7 +3844,7 @@
         <v>311</v>
       </c>
       <c r="B313">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -3852,7 +3852,7 @@
         <v>312</v>
       </c>
       <c r="B314">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -3860,7 +3860,7 @@
         <v>313</v>
       </c>
       <c r="B315">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -3868,7 +3868,7 @@
         <v>314</v>
       </c>
       <c r="B316">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -3876,7 +3876,7 @@
         <v>315</v>
       </c>
       <c r="B317">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -3884,7 +3884,7 @@
         <v>316</v>
       </c>
       <c r="B318">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -3892,7 +3892,7 @@
         <v>317</v>
       </c>
       <c r="B319">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -3900,7 +3900,7 @@
         <v>318</v>
       </c>
       <c r="B320">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -3908,7 +3908,7 @@
         <v>319</v>
       </c>
       <c r="B321">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -3916,7 +3916,7 @@
         <v>320</v>
       </c>
       <c r="B322">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -3924,7 +3924,7 @@
         <v>321</v>
       </c>
       <c r="B323">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -3932,7 +3932,7 @@
         <v>322</v>
       </c>
       <c r="B324">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>